<commit_message>
update to 3 sensors, 3 buttons, and latest pinouts
</commit_message>
<xml_diff>
--- a/spreadsheets/rp-pico-2-pin-planner-artcar-3sonar.xlsx
+++ b/spreadsheets/rp-pico-2-pin-planner-artcar-3sonar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bradcarlile/Documents/GitHub/artcar-ultrasonic-dist-rp2/spreadsheets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD164CC0-11E7-B847-B764-C4DCDCDC466A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E15B5F49-B73E-F343-A445-DB3B9BA1E95E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7460" yWindow="-21100" windowWidth="24520" windowHeight="20120" xr2:uid="{9994E188-9327-AB46-AF3F-8738237FB097}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="107">
   <si>
     <t>gp0</t>
   </si>
@@ -354,6 +354,9 @@
   </si>
   <si>
     <t>bme680(#77), bmp390(#76)</t>
+  </si>
+  <si>
+    <t>Button3</t>
   </si>
 </sst>
 </file>
@@ -650,124 +653,133 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -776,7 +788,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -785,19 +797,10 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1145,879 +1148,888 @@
   </sheetPr>
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="176" workbookViewId="0">
-      <selection activeCell="G41" sqref="G41"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="176" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="18" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.140625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="8.5703125" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" style="4" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.28515625" style="4" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="2.85546875" style="4" customWidth="1"/>
-    <col min="7" max="7" width="25.7109375" style="5" customWidth="1"/>
-    <col min="8" max="8" width="16.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="24.7109375" style="5" customWidth="1"/>
-    <col min="10" max="16384" width="10.7109375" style="5"/>
+    <col min="1" max="1" width="7.140625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.5703125" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.7109375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="2.85546875" style="2" customWidth="1"/>
+    <col min="7" max="7" width="25.7109375" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="24.7109375" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="10.7109375" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="41" t="s">
         <v>76</v>
       </c>
-      <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
-      <c r="E1" s="3"/>
-      <c r="G1" s="5" t="s">
+      <c r="C1" s="41"/>
+      <c r="D1" s="41"/>
+      <c r="E1" s="42"/>
+      <c r="G1" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="H1" s="6">
+      <c r="H1" s="4">
         <v>45597</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="G2" s="7" t="s">
+      <c r="G2" s="5" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B3" s="4">
+      <c r="B3" s="2">
         <v>0</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3" s="2">
         <v>1</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="2">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="B4" s="8"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="8"/>
+      <c r="B4" s="6"/>
+      <c r="C4" s="6"/>
+      <c r="D4" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9" t="s">
+      <c r="B5" s="7"/>
+      <c r="C5" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="10"/>
+      <c r="D5" s="8"/>
     </row>
     <row r="6" spans="1:9" ht="39" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6" t="s">
         <v>104</v>
       </c>
-      <c r="D6" s="10"/>
+      <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:9" ht="20" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
+      <c r="A7" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="6" t="s">
         <v>48</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:9" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="10" t="s">
         <v>73</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="10" t="s">
         <v>74</v>
       </c>
-      <c r="I8" s="12" t="s">
+      <c r="I8" s="10" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="13">
+      <c r="A9" s="11">
         <v>1</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="12" t="s">
         <v>0</v>
       </c>
-      <c r="C9" s="15" t="s">
+      <c r="C9" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="G9" s="5" t="s">
+      <c r="G9" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H9" s="4" t="s">
+      <c r="H9" s="2" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="16">
         <v>2</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="17" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="20" t="s">
+      <c r="C10" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="D10" s="21" t="s">
+      <c r="D10" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="G10" s="5" t="s">
+      <c r="G10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H10" s="4" t="s">
+      <c r="H10" s="2" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
+      <c r="A11" s="16">
         <v>3</v>
       </c>
-      <c r="B11" s="23" t="s">
+      <c r="B11" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E11" s="24"/>
+      <c r="E11" s="22"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="16">
         <v>4</v>
       </c>
-      <c r="B12" s="19" t="s">
+      <c r="B12" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C12" s="20" t="s">
+      <c r="C12" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D12" s="21" t="s">
+      <c r="D12" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E12" s="24"/>
-      <c r="F12" s="4" t="s">
+      <c r="E12" s="22"/>
+      <c r="F12" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G12" s="5" t="s">
+      <c r="G12" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="H12" s="25" t="s">
+      <c r="H12" s="23" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="16">
         <v>5</v>
       </c>
-      <c r="B13" s="19" t="s">
+      <c r="B13" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="20" t="s">
+      <c r="C13" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D13" s="21" t="s">
+      <c r="D13" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E13" s="24"/>
-      <c r="F13" s="4" t="s">
+      <c r="E13" s="22"/>
+      <c r="F13" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="23" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+      <c r="A14" s="16">
         <v>6</v>
       </c>
-      <c r="B14" s="19" t="s">
+      <c r="B14" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C14" s="20" t="s">
+      <c r="C14" s="18" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="21" t="s">
+      <c r="D14" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F14" s="4" t="s">
+      <c r="F14" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G14" s="26" t="s">
+      <c r="G14" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H14" s="4" t="s">
+      <c r="H14" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="I14" s="26" t="s">
+      <c r="I14" s="24" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="A15" s="16">
         <v>7</v>
       </c>
-      <c r="B15" s="19" t="s">
+      <c r="B15" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C15" s="20" t="s">
+      <c r="C15" s="18" t="s">
         <v>32</v>
       </c>
-      <c r="D15" s="21" t="s">
+      <c r="D15" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="4" t="s">
+      <c r="F15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="G15" s="26" t="s">
+      <c r="G15" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="H15" s="4" t="s">
+      <c r="H15" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="I15" s="26" t="s">
+      <c r="I15" s="24" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+      <c r="A16" s="16">
         <v>8</v>
       </c>
-      <c r="B16" s="23" t="s">
+      <c r="B16" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E16" s="24"/>
+      <c r="E16" s="22"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+      <c r="A17" s="16">
         <v>9</v>
       </c>
-      <c r="B17" s="19" t="s">
+      <c r="B17" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D17" s="21" t="s">
+      <c r="D17" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E17" s="24"/>
-      <c r="F17" s="4" t="s">
+      <c r="E17" s="22"/>
+      <c r="F17" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G17" s="5" t="s">
+      <c r="G17" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="H17" s="4" t="s">
+      <c r="H17" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
+      <c r="A18" s="16">
         <v>10</v>
       </c>
-      <c r="B18" s="19" t="s">
+      <c r="B18" s="17" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="18" t="s">
         <v>31</v>
       </c>
-      <c r="D18" s="21" t="s">
+      <c r="D18" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E18" s="24"/>
-      <c r="F18" s="4" t="s">
+      <c r="E18" s="22"/>
+      <c r="F18" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G18" s="5" t="s">
+      <c r="G18" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="H18" s="4" t="s">
+      <c r="H18" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="A19" s="16">
         <v>11</v>
       </c>
-      <c r="B19" s="19" t="s">
+      <c r="B19" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="C19" s="20" t="s">
+      <c r="C19" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D19" s="21" t="s">
+      <c r="D19" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="F19" s="4" t="s">
+      <c r="F19" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G19" s="5" t="s">
+      <c r="G19" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="H19" s="4" t="s">
+      <c r="H19" s="2" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+      <c r="A20" s="16">
         <v>12</v>
       </c>
-      <c r="B20" s="19" t="s">
+      <c r="B20" s="17" t="s">
         <v>9</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D20" s="21" t="s">
+      <c r="D20" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="G20" s="5" t="s">
+      <c r="G20" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="2" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="16">
         <v>13</v>
       </c>
-      <c r="B21" s="23" t="s">
+      <c r="B21" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E21" s="24"/>
+      <c r="E21" s="22"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+      <c r="A22" s="16">
         <v>14</v>
       </c>
-      <c r="B22" s="19" t="s">
+      <c r="B22" s="17" t="s">
         <v>10</v>
       </c>
-      <c r="C22" s="20" t="s">
+      <c r="C22" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E22" s="24"/>
-      <c r="F22" s="4" t="s">
+      <c r="E22" s="22"/>
+      <c r="F22" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G22" s="5" t="s">
+      <c r="G22" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="2" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
+      <c r="A23" s="16">
         <v>15</v>
       </c>
-      <c r="B23" s="19" t="s">
+      <c r="B23" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="20" t="s">
+      <c r="C23" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D23" s="21" t="s">
+      <c r="D23" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E23" s="24"/>
-      <c r="F23" s="4" t="s">
+      <c r="E23" s="22"/>
+      <c r="F23" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G23" s="5" t="s">
+      <c r="G23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="2" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18">
+      <c r="A24" s="16">
         <v>16</v>
       </c>
-      <c r="B24" s="19" t="s">
+      <c r="B24" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="C24" s="20" t="s">
+      <c r="C24" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D24" s="21" t="s">
+      <c r="D24" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="20" t="s">
         <v>43</v>
       </c>
-      <c r="F24" s="4" t="s">
+      <c r="F24" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G24" s="5" t="s">
+      <c r="G24" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="H24" s="4" t="s">
+      <c r="H24" s="2" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
+      <c r="A25" s="16">
         <v>17</v>
       </c>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>13</v>
       </c>
-      <c r="C25" s="20" t="s">
+      <c r="C25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D25" s="21" t="s">
+      <c r="D25" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F25" s="4" t="s">
+      <c r="F25" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G25" s="5" t="s">
+      <c r="G25" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="H25" s="4" t="s">
+      <c r="H25" s="2" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="A26" s="16">
         <v>18</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="21" t="s">
         <v>26</v>
       </c>
-      <c r="E26" s="24"/>
+      <c r="E26" s="22"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
+      <c r="A27" s="16">
         <v>19</v>
       </c>
-      <c r="B27" s="19" t="s">
+      <c r="B27" s="17" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D27" s="21" t="s">
+      <c r="D27" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E27" s="24"/>
+      <c r="E27" s="22"/>
     </row>
     <row r="28" spans="1:8" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="27">
+      <c r="A28" s="25">
         <v>20</v>
       </c>
-      <c r="B28" s="28" t="s">
+      <c r="B28" s="26" t="s">
         <v>15</v>
       </c>
-      <c r="C28" s="29" t="s">
+      <c r="C28" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="28" t="s">
         <v>42</v>
       </c>
-      <c r="E28" s="31"/>
-    </row>
-    <row r="29" spans="1:8" s="34" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="32"/>
-      <c r="B29" s="33"/>
-      <c r="C29" s="32"/>
-      <c r="D29" s="32"/>
-      <c r="E29" s="32"/>
-      <c r="H29" s="32"/>
+      <c r="E28" s="29"/>
+      <c r="F28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="G28" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="H28" s="23" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" s="32" customFormat="1" ht="19" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="30"/>
+      <c r="B29" s="31"/>
+      <c r="C29" s="30"/>
+      <c r="D29" s="30"/>
+      <c r="E29" s="30"/>
+      <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="A30" s="2">
         <v>21</v>
       </c>
-      <c r="B30" s="35" t="s">
+      <c r="B30" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="C30" s="15" t="s">
+      <c r="C30" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="D30" s="16" t="s">
+      <c r="D30" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="E30" s="17" t="s">
+      <c r="E30" s="15" t="s">
         <v>43</v>
       </c>
-      <c r="F30" s="4" t="s">
+      <c r="F30" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G30" s="5" t="s">
+      <c r="G30" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H30" s="4" t="s">
+      <c r="H30" s="2" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="A31" s="2">
         <v>22</v>
       </c>
-      <c r="B31" s="36" t="s">
+      <c r="B31" s="34" t="s">
         <v>24</v>
       </c>
-      <c r="C31" s="20" t="s">
+      <c r="C31" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="21" t="s">
+      <c r="D31" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="20" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="4" t="s">
+      <c r="F31" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G31" s="5" t="s">
+      <c r="G31" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="H31" s="4" t="s">
+      <c r="H31" s="2" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="A32" s="2">
         <v>23</v>
       </c>
-      <c r="B32" s="37" t="s">
+      <c r="B32" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E32" s="24"/>
+      <c r="E32" s="22"/>
     </row>
     <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="A33" s="2">
         <v>24</v>
       </c>
-      <c r="B33" s="36" t="s">
+      <c r="B33" s="34" t="s">
         <v>23</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="D33" s="21" t="s">
+      <c r="D33" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E33" s="24"/>
-      <c r="F33" s="4" t="s">
+      <c r="E33" s="22"/>
+      <c r="F33" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G33" s="5" t="s">
+      <c r="G33" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="H33" s="25" t="s">
+      <c r="H33" s="23" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="A34" s="2">
         <v>25</v>
       </c>
-      <c r="B34" s="36" t="s">
+      <c r="B34" s="34" t="s">
         <v>22</v>
       </c>
-      <c r="C34" s="20" t="s">
+      <c r="C34" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="D34" s="21" t="s">
+      <c r="D34" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="4" t="s">
+      <c r="E34" s="22"/>
+      <c r="F34" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G34" s="5" t="s">
+      <c r="G34" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" s="4">
+      <c r="A35" s="2">
         <v>26</v>
       </c>
-      <c r="B35" s="36" t="s">
+      <c r="B35" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D35" s="21" t="s">
+      <c r="D35" s="19" t="s">
         <v>39</v>
       </c>
-      <c r="E35" s="24"/>
-      <c r="F35" s="4" t="s">
+      <c r="E35" s="22"/>
+      <c r="F35" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G35" s="5" t="s">
+      <c r="G35" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="H35" s="25" t="s">
+      <c r="H35" s="23" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" s="4">
+      <c r="A36" s="2">
         <v>27</v>
       </c>
-      <c r="B36" s="36" t="s">
+      <c r="B36" s="34" t="s">
         <v>20</v>
       </c>
-      <c r="D36" s="21" t="s">
+      <c r="D36" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="E36" s="24"/>
-      <c r="F36" s="4" t="s">
+      <c r="E36" s="22"/>
+      <c r="F36" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G36" s="5" t="s">
+      <c r="G36" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="H36" s="25" t="s">
+      <c r="H36" s="23" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="A37" s="2">
         <v>28</v>
       </c>
-      <c r="B37" s="37" t="s">
+      <c r="B37" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="24"/>
+      <c r="E37" s="22"/>
     </row>
     <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="A38" s="2">
         <v>29</v>
       </c>
-      <c r="B38" s="36" t="s">
+      <c r="B38" s="34" t="s">
         <v>19</v>
       </c>
-      <c r="E38" s="24"/>
-      <c r="G38" s="5" t="s">
+      <c r="E38" s="22"/>
+      <c r="G38" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="H38" s="25" t="s">
+      <c r="H38" s="23" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" s="4">
+      <c r="A39" s="2">
         <v>30</v>
       </c>
-      <c r="B39" s="38" t="s">
+      <c r="B39" s="36" t="s">
         <v>36</v>
       </c>
-      <c r="E39" s="24"/>
+      <c r="E39" s="22"/>
     </row>
     <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" s="4">
+      <c r="A40" s="2">
         <v>31</v>
       </c>
-      <c r="B40" s="36" t="s">
+      <c r="B40" s="34" t="s">
         <v>18</v>
       </c>
-      <c r="C40" s="39" t="s">
+      <c r="C40" s="37" t="s">
         <v>70</v>
       </c>
-      <c r="D40" s="21" t="s">
+      <c r="D40" s="19" t="s">
         <v>41</v>
       </c>
-      <c r="E40" s="24"/>
-      <c r="F40" s="4" t="s">
+      <c r="E40" s="22"/>
+      <c r="F40" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G40" s="5" t="s">
+      <c r="G40" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H40" s="4" t="s">
+      <c r="H40" s="2" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" s="4">
+      <c r="A41" s="2">
         <v>32</v>
       </c>
-      <c r="B41" s="36" t="s">
+      <c r="B41" s="34" t="s">
         <v>17</v>
       </c>
-      <c r="C41" s="39" t="s">
+      <c r="C41" s="37" t="s">
         <v>69</v>
       </c>
-      <c r="D41" s="21" t="s">
+      <c r="D41" s="19" t="s">
         <v>42</v>
       </c>
-      <c r="E41" s="24"/>
-      <c r="F41" s="4" t="s">
+      <c r="E41" s="22"/>
+      <c r="F41" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G41" s="5" t="s">
+      <c r="G41" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="H41" s="4" t="s">
+      <c r="H41" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="J41" s="25"/>
+      <c r="J41" s="23"/>
     </row>
     <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" s="4">
+      <c r="A42" s="2">
         <v>33</v>
       </c>
-      <c r="B42" s="37" t="s">
+      <c r="B42" s="35" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="39" t="s">
+      <c r="C42" s="37" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="24"/>
-      <c r="G42" s="5" t="s">
+      <c r="E42" s="22"/>
+      <c r="G42" s="3" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" s="4">
+      <c r="A43" s="2">
         <v>34</v>
       </c>
-      <c r="B43" s="36" t="s">
+      <c r="B43" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C43" s="39" t="s">
+      <c r="C43" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="E43" s="24"/>
-      <c r="F43" s="4" t="s">
+      <c r="E43" s="22"/>
+      <c r="F43" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="G43" s="5" t="s">
+      <c r="G43" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="H43" s="25" t="s">
+      <c r="H43" s="23" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" s="4">
+      <c r="A44" s="2">
         <v>35</v>
       </c>
-      <c r="B44" s="18"/>
-      <c r="C44" s="39" t="s">
+      <c r="B44" s="16"/>
+      <c r="C44" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="E44" s="24"/>
+      <c r="E44" s="22"/>
     </row>
     <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" s="4">
+      <c r="A45" s="2">
         <v>36</v>
       </c>
-      <c r="B45" s="40" t="s">
+      <c r="B45" s="43" t="s">
         <v>102</v>
       </c>
-      <c r="C45" s="41"/>
-      <c r="D45" s="41"/>
-      <c r="E45" s="42"/>
+      <c r="C45" s="44"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="45"/>
     </row>
     <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" s="4">
+      <c r="A46" s="2">
         <v>37</v>
       </c>
-      <c r="B46" s="40" t="s">
+      <c r="B46" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="C46" s="41"/>
-      <c r="D46" s="41"/>
-      <c r="E46" s="42"/>
+      <c r="C46" s="44"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="45"/>
     </row>
     <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" s="4">
+      <c r="A47" s="2">
         <v>38</v>
       </c>
-      <c r="B47" s="43" t="s">
+      <c r="B47" s="46" t="s">
         <v>26</v>
       </c>
-      <c r="C47" s="44"/>
-      <c r="D47" s="44"/>
-      <c r="E47" s="45"/>
-      <c r="G47" s="5" t="s">
+      <c r="C47" s="47"/>
+      <c r="D47" s="47"/>
+      <c r="E47" s="48"/>
+      <c r="G47" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" s="4">
+      <c r="A48" s="2">
         <v>39</v>
       </c>
-      <c r="B48" s="46" t="s">
+      <c r="B48" s="49" t="s">
         <v>101</v>
       </c>
-      <c r="C48" s="47"/>
-      <c r="D48" s="47"/>
-      <c r="E48" s="48"/>
+      <c r="C48" s="50"/>
+      <c r="D48" s="50"/>
+      <c r="E48" s="51"/>
     </row>
     <row r="49" spans="1:5" ht="19" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A49" s="4">
+      <c r="A49" s="2">
         <v>40</v>
       </c>
-      <c r="B49" s="49" t="s">
+      <c r="B49" s="38" t="s">
         <v>103</v>
       </c>
-      <c r="C49" s="50"/>
-      <c r="D49" s="50"/>
-      <c r="E49" s="51"/>
+      <c r="C49" s="39"/>
+      <c r="D49" s="39"/>
+      <c r="E49" s="40"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B50" s="25"/>
+      <c r="B50" s="23"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B51" s="25"/>
+      <c r="B51" s="23"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B52" s="25"/>
+      <c r="B52" s="23"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="B53" s="25"/>
+      <c r="B53" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>